<commit_message>
final commit for the app
</commit_message>
<xml_diff>
--- a/air_quality/data_poland/dummy_data/pred.xlsx
+++ b/air_quality/data_poland/dummy_data/pred.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ernest_pokropek/Desktop/uni/scalable_ml/air_quality/data_poland/dummy_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB0B1267-DAE3-CF49-A56F-A9B8FE6480C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8996A7CC-C56E-194D-8804-EFB22870FDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="2420" windowWidth="27240" windowHeight="16440" xr2:uid="{A55A2172-9FBC-404D-8797-928673F3096C}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>city_name</t>
-  </si>
-  <si>
     <t>biala_podlaska</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>lomza</t>
+  </si>
+  <si>
+    <t>city</t>
   </si>
 </sst>
 </file>
@@ -456,15 +456,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B934D358-022A-264E-A86D-FCC152D521FC}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1">
         <v>44938</v>
@@ -490,7 +488,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>36</v>
@@ -516,7 +514,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>58</v>
@@ -542,7 +540,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>23</v>
@@ -568,7 +566,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>57</v>
@@ -594,7 +592,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -620,7 +618,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -646,7 +644,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>53</v>
@@ -672,7 +670,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -698,7 +696,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>33</v>
@@ -724,7 +722,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>57</v>
@@ -750,7 +748,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>22</v>
@@ -776,7 +774,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>31</v>
@@ -802,7 +800,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>54</v>
@@ -828,7 +826,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>17</v>
@@ -854,7 +852,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>33</v>
@@ -880,7 +878,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>51</v>
@@ -906,7 +904,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>19</v>
@@ -932,7 +930,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>31</v>
@@ -958,7 +956,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>60</v>
@@ -984,7 +982,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>24</v>
@@ -1010,7 +1008,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>36</v>

</xml_diff>